<commit_message>
Fix validation status - all intersections now show NOT_STARTED
- Updated interpret_validation() to return NOT_STARTED for all
- Regenerated INTERSECTION_STATUS_FINAL.xlsx
- Regenerated embedded-data.js with corrected validation status

https://claude.ai/code/session_01MD92mQo6vT3XosTWnx29qJ
</commit_message>
<xml_diff>
--- a/data-import/INTERSECTION_STATUS_FINAL.xlsx
+++ b/data-import/INTERSECTION_STATUS_FINAL.xlsx
@@ -1429,9 +1429,9 @@
           <t>Idoneo</t>
         </is>
       </c>
-      <c r="M13" s="5" t="inlineStr">
-        <is>
-          <t>IN_VERIFICATION</t>
+      <c r="M13" s="4" t="inlineStr">
+        <is>
+          <t>NOT_STARTED</t>
         </is>
       </c>
       <c r="N13" s="2" t="inlineStr">
@@ -17199,9 +17199,9 @@
           <t>Idoneo</t>
         </is>
       </c>
-      <c r="M13" s="5" t="inlineStr">
-        <is>
-          <t>IN_VERIFICATION</t>
+      <c r="M13" s="4" t="inlineStr">
+        <is>
+          <t>NOT_STARTED</t>
         </is>
       </c>
       <c r="N13" s="2" t="inlineStr">

</xml_diff>